<commit_message>
Update Portfolio Optimization Tool.xlsx
update heat map conditional formatting
</commit_message>
<xml_diff>
--- a/Portfolio Optimization Tool.xlsx
+++ b/Portfolio Optimization Tool.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanlupinski/PycharmProjects/Finance/Portfolio Optimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C873D3E-7CF0-D14D-9DA2-F760F3830ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7C2D77-B9C9-5749-96C5-F6A2A3A87EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Portfolio" sheetId="1" r:id="rId1"/>
@@ -348,7 +348,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -609,19 +609,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -655,7 +642,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="6" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -701,24 +688,15 @@
     <xf numFmtId="10" fontId="6" fillId="12" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="6" fillId="12" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="12" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="13" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="6" fillId="13" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="6" fillId="13" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="6" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="6" fillId="12" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="6" fillId="9" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="6" fillId="9" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="4" fillId="10" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -739,6 +717,7 @@
     <xf numFmtId="0" fontId="5" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -769,7 +748,6 @@
     <xf numFmtId="165" fontId="8" fillId="15" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="13" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Heading" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -785,7 +763,475 @@
     <cellStyle name="Untitled6" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Untitled7" xfId="11" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="56">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF006600"/>
+          <bgColor rgb="FF006600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF006600"/>
+          <bgColor rgb="FF006600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF006600"/>
+          <bgColor rgb="FF006600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF006600"/>
+          <bgColor rgb="FF006600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF006600"/>
+          <bgColor rgb="FF006600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF006600"/>
+          <bgColor rgb="FF006600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF006600"/>
+          <bgColor rgb="FF006600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF006600"/>
+          <bgColor rgb="FF006600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF006600"/>
+          <bgColor rgb="FF006600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF006600"/>
+          <bgColor rgb="FF006600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF006600"/>
+          <bgColor rgb="FF006600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF006600"/>
+          <bgColor rgb="FF006600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF006600"/>
+          <bgColor rgb="FF006600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF006600"/>
+          <bgColor rgb="FF006600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF006600"/>
+          <bgColor rgb="FF006600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF006600"/>
+          <bgColor rgb="FF006600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF006600"/>
+          <bgColor rgb="FF006600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF006600"/>
+          <bgColor rgb="FF006600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF006600"/>
+          <bgColor rgb="FF006600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF006600"/>
+          <bgColor rgb="FF006600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF006600"/>
+          <bgColor rgb="FF006600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF006600"/>
+          <bgColor rgb="FF006600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF006600"/>
+          <bgColor rgb="FF006600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF006600"/>
+          <bgColor rgb="FF006600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF006600"/>
+          <bgColor rgb="FF006600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF006600"/>
+          <bgColor rgb="FF006600"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1927,8 +2373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="R17" sqref="R17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1950,20 +2396,20 @@
   <sheetData>
     <row r="1" spans="2:16" ht="14.5" customHeight="1" thickBot="1"/>
     <row r="2" spans="2:16" ht="17" thickBot="1">
-      <c r="G2" s="45" t="s">
+      <c r="G2" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="47">
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="45">
         <f>INDEX('Price Data'!$A$2:$A$265,COUNT('Price Data'!$A$2:$A$265))</f>
         <v>44712</v>
       </c>
-      <c r="K2" s="48">
+      <c r="K2" s="46">
         <f>INDEX('Price Data'!$L$2:$L$255,COUNT('Price Data'!$L$2:$L$255))</f>
         <v>99.069999694824205</v>
       </c>
-      <c r="L2" s="39" t="s">
+      <c r="L2" s="37" t="s">
         <v>0</v>
       </c>
       <c r="M2" s="9" t="s">
@@ -1972,56 +2418,56 @@
       <c r="N2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="O2" s="41" t="s">
+      <c r="O2" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="P2" s="43" t="s">
+      <c r="P2" s="41" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="2:16">
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="36" t="s">
+      <c r="G3" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="37" t="s">
+      <c r="H3" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="37" t="s">
+      <c r="I3" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="37" t="s">
+      <c r="J3" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="38" t="s">
+      <c r="K3" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="40"/>
+      <c r="L3" s="38"/>
       <c r="M3" s="11" t="s">
         <v>15</v>
       </c>
       <c r="N3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="42"/>
-      <c r="P3" s="44"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="42"/>
     </row>
     <row r="4" spans="2:16">
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="27" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -2034,11 +2480,11 @@
         <f t="shared" ref="E4:E14" si="0">IF(P4="buy",0.1,0)</f>
         <v>0</v>
       </c>
-      <c r="F4" s="31">
+      <c r="F4" s="28">
         <f t="shared" ref="F4:F15" si="1">D4+E4</f>
         <v>0.05</v>
       </c>
-      <c r="G4" s="24">
+      <c r="G4" s="22">
         <f>'Performance Data'!$B$2</f>
         <v>-5.9891763000000002E-3</v>
       </c>
@@ -2062,11 +2508,11 @@
         <f t="shared" ref="L4:L14" si="3">_xlfn.RANK.EQ(K4,$K$4:$K$14,0)</f>
         <v>10</v>
       </c>
-      <c r="M4" s="21">
+      <c r="M4" s="19">
         <f>INDEX('Price Data'!$B$2:$B$265,COUNT('Price Data'!$B$2:$B$265))</f>
         <v>146.05000305175699</v>
       </c>
-      <c r="N4" s="22">
+      <c r="N4" s="20">
         <f>'200D SMA'!$B$2</f>
         <v>170.661000213623</v>
       </c>
@@ -2080,7 +2526,7 @@
       </c>
     </row>
     <row r="5" spans="2:16">
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="27" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
@@ -2093,11 +2539,11 @@
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="F5" s="31">
+      <c r="F5" s="28">
         <f t="shared" si="1"/>
         <v>0.15000000000000002</v>
       </c>
-      <c r="G5" s="24">
+      <c r="G5" s="22">
         <f>'Performance Data'!$C$2</f>
         <v>2.4093812799999999E-2</v>
       </c>
@@ -2121,11 +2567,11 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="M5" s="21">
+      <c r="M5" s="19">
         <f>INDEX('Price Data'!$C$2:$C$265,COUNT('Price Data'!$C$2:$C$265))</f>
         <v>144.08999633789</v>
       </c>
-      <c r="N5" s="22">
+      <c r="N5" s="20">
         <f>'200D SMA'!$C$2</f>
         <v>143.467700042724</v>
       </c>
@@ -2139,7 +2585,7 @@
       </c>
     </row>
     <row r="6" spans="2:16">
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="27" t="s">
         <v>44</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -2152,11 +2598,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F6" s="31">
+      <c r="F6" s="28">
         <f t="shared" si="1"/>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="G6" s="24">
+      <c r="G6" s="22">
         <f>'Performance Data'!$D$2</f>
         <v>1.6338675399999999E-2</v>
       </c>
@@ -2180,11 +2626,11 @@
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="M6" s="21">
+      <c r="M6" s="19">
         <f>INDEX('Price Data'!$D$2:$D$265,COUNT('Price Data'!$D$2:$D$265))</f>
         <v>54.740001678466797</v>
       </c>
-      <c r="N6" s="22">
+      <c r="N6" s="20">
         <f>'200D SMA'!$D$2</f>
         <v>59.593499927520703</v>
       </c>
@@ -2198,7 +2644,7 @@
       </c>
     </row>
     <row r="7" spans="2:16">
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="27" t="s">
         <v>45</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -2211,11 +2657,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F7" s="31">
+      <c r="F7" s="28">
         <f t="shared" si="1"/>
         <v>2.2499999999999999E-2</v>
       </c>
-      <c r="G7" s="24">
+      <c r="G7" s="22">
         <f>'Performance Data'!$E$2</f>
         <v>4.6040693000000002E-3</v>
       </c>
@@ -2239,11 +2685,11 @@
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="M7" s="21">
+      <c r="M7" s="19">
         <f>INDEX('Price Data'!$E$2:$E$265,COUNT('Price Data'!$E$2:$E$265))</f>
         <v>43.639999389648402</v>
       </c>
-      <c r="N7" s="22">
+      <c r="N7" s="20">
         <f>'200D SMA'!$E$2</f>
         <v>48.427849941253598</v>
       </c>
@@ -2257,7 +2703,7 @@
       </c>
     </row>
     <row r="8" spans="2:16">
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="27" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -2270,11 +2716,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F8" s="31">
+      <c r="F8" s="28">
         <f t="shared" si="1"/>
         <v>8.8999999999999996E-2</v>
       </c>
-      <c r="G8" s="24">
+      <c r="G8" s="22">
         <f>'Performance Data'!$F$2</f>
         <v>1.07882464E-2</v>
       </c>
@@ -2298,11 +2744,11 @@
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="M8" s="21">
+      <c r="M8" s="19">
         <f>INDEX('Price Data'!$F$2:$F$265,COUNT('Price Data'!$F$2:$F$265))</f>
         <v>82.449996948242102</v>
       </c>
-      <c r="N8" s="22">
+      <c r="N8" s="20">
         <f>'200D SMA'!$F$2</f>
         <v>90.086999969482406</v>
       </c>
@@ -2316,7 +2762,7 @@
       </c>
     </row>
     <row r="9" spans="2:16">
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="27" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -2329,11 +2775,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F9" s="31">
+      <c r="F9" s="28">
         <f t="shared" si="1"/>
         <v>6.7500000000000004E-2</v>
       </c>
-      <c r="G9" s="24">
+      <c r="G9" s="22">
         <f>'Performance Data'!$G$2</f>
         <v>-2.2091117899999999E-2</v>
       </c>
@@ -2357,11 +2803,11 @@
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="M9" s="21">
+      <c r="M9" s="19">
         <f>INDEX('Price Data'!$G$2:$G$265,COUNT('Price Data'!$G$2:$G$265))</f>
         <v>71.269996643066406</v>
       </c>
-      <c r="N9" s="22">
+      <c r="N9" s="20">
         <f>'200D SMA'!$G$2</f>
         <v>84.335749969482407</v>
       </c>
@@ -2375,7 +2821,7 @@
       </c>
     </row>
     <row r="10" spans="2:16">
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="27" t="s">
         <v>27</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -2388,11 +2834,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F10" s="31">
+      <c r="F10" s="28">
         <f t="shared" si="1"/>
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="G10" s="24">
+      <c r="G10" s="22">
         <f>'Performance Data'!$H$2</f>
         <v>-7.4759207999999999E-3</v>
       </c>
@@ -2416,11 +2862,11 @@
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="M10" s="21">
+      <c r="M10" s="19">
         <f>INDEX('Price Data'!$H$2:$H$265,COUNT('Price Data'!$H$2:$H$265))</f>
         <v>50.450000762939403</v>
       </c>
-      <c r="N10" s="22">
+      <c r="N10" s="20">
         <f>'200D SMA'!$H$2</f>
         <v>54.796000022888101</v>
       </c>
@@ -2434,7 +2880,7 @@
       </c>
     </row>
     <row r="11" spans="2:16">
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="27" t="s">
         <v>29</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -2447,11 +2893,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F11" s="31">
+      <c r="F11" s="28">
         <f t="shared" si="1"/>
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="G11" s="24">
+      <c r="G11" s="22">
         <f>'Performance Data'!$I$2</f>
         <v>5.3286059999999996E-3</v>
       </c>
@@ -2475,11 +2921,11 @@
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="M11" s="21">
+      <c r="M11" s="19">
         <f>INDEX('Price Data'!$I$2:$I$265,COUNT('Price Data'!$I$2:$I$265))</f>
         <v>50.939998626708899</v>
       </c>
-      <c r="N11" s="22">
+      <c r="N11" s="20">
         <f>'200D SMA'!$I$2</f>
         <v>51.608049964904701</v>
       </c>
@@ -2493,7 +2939,7 @@
       </c>
     </row>
     <row r="12" spans="2:16">
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="27" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -2506,11 +2952,11 @@
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="F12" s="31">
+      <c r="F12" s="28">
         <f t="shared" si="1"/>
         <v>0.125</v>
       </c>
-      <c r="G12" s="24">
+      <c r="G12" s="22">
         <f>'Performance Data'!$J$2</f>
         <v>4.6131439099999998E-2</v>
       </c>
@@ -2534,11 +2980,11 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="M12" s="21">
+      <c r="M12" s="19">
         <f>INDEX('Price Data'!$J$2:$J$265,COUNT('Price Data'!$J$2:$J$265))</f>
         <v>28.799999237060501</v>
       </c>
-      <c r="N12" s="22">
+      <c r="N12" s="20">
         <f>'200D SMA'!$J$2</f>
         <v>22.896499977111802</v>
       </c>
@@ -2552,7 +2998,7 @@
       </c>
     </row>
     <row r="13" spans="2:16">
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="27" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -2565,11 +3011,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F13" s="31">
+      <c r="F13" s="28">
         <f t="shared" si="1"/>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="G13" s="24">
+      <c r="G13" s="22">
         <f>'Performance Data'!$K$2</f>
         <v>-3.2463983199999998E-2</v>
       </c>
@@ -2593,11 +3039,11 @@
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="M13" s="21">
+      <c r="M13" s="19">
         <f>INDEX('Price Data'!$K$2:$K$265,COUNT('Price Data'!$K$2:$K$265))</f>
         <v>34.869998931884702</v>
       </c>
-      <c r="N13" s="22">
+      <c r="N13" s="20">
         <f>'200D SMA'!$K$2</f>
         <v>34.975750102996798</v>
       </c>
@@ -2611,7 +3057,7 @@
       </c>
     </row>
     <row r="14" spans="2:16" ht="17" thickBot="1">
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="27" t="s">
         <v>35</v>
       </c>
       <c r="C14" s="1" t="s">
@@ -2624,27 +3070,27 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F14" s="31">
+      <c r="F14" s="28">
         <f t="shared" si="1"/>
         <v>2.2499999999999999E-2</v>
       </c>
-      <c r="G14" s="25">
+      <c r="G14" s="22">
         <f>'Performance Data'!$L$2</f>
         <v>-4.6853979499999997E-2</v>
       </c>
-      <c r="H14" s="19">
+      <c r="H14" s="6">
         <f>'Performance Data'!$L$3</f>
         <v>-3.3840464100000002E-2</v>
       </c>
-      <c r="I14" s="19">
+      <c r="I14" s="6">
         <f>'Performance Data'!$L$4</f>
         <v>-7.1856832699999998E-2</v>
       </c>
-      <c r="J14" s="19">
+      <c r="J14" s="6">
         <f>'Performance Data'!$L$5</f>
         <v>-1.0511603999999999E-3</v>
       </c>
-      <c r="K14" s="20">
+      <c r="K14" s="18">
         <f t="shared" si="2"/>
         <v>-3.8400609174999996E-2</v>
       </c>
@@ -2652,11 +3098,11 @@
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="M14" s="49">
+      <c r="M14" s="36">
         <f>INDEX('Price Data'!$L$2:$L$265,COUNT('Price Data'!$L$2:$L$265))</f>
         <v>99.069999694824205</v>
       </c>
-      <c r="N14" s="23">
+      <c r="N14" s="21">
         <f>'200D SMA'!$L$2</f>
         <v>106.527500190734</v>
       </c>
@@ -2670,7 +3116,7 @@
       </c>
     </row>
     <row r="15" spans="2:16">
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="27" t="s">
         <v>37</v>
       </c>
       <c r="C15" s="1" t="s">
@@ -2683,25 +3129,25 @@
         <f>0.5-SUM(E4:E14)</f>
         <v>0.3</v>
       </c>
-      <c r="F15" s="31">
+      <c r="F15" s="28">
         <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
     </row>
     <row r="16" spans="2:16" ht="17" thickBot="1">
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="34">
+      <c r="C16" s="30"/>
+      <c r="D16" s="31">
         <f>SUM(D4:D15)</f>
         <v>0.50000000000000011</v>
       </c>
-      <c r="E16" s="34">
+      <c r="E16" s="31">
         <f>SUM(E4:E15)</f>
         <v>0.5</v>
       </c>
-      <c r="F16" s="35">
+      <c r="F16" s="32">
         <f>SUM(F4:F15)</f>
         <v>1</v>
       </c>
@@ -2715,31 +3161,31 @@
     <mergeCell ref="J2:K2"/>
   </mergeCells>
   <conditionalFormatting sqref="L2 L4:L14">
-    <cfRule type="cellIs" dxfId="3" priority="14" stopIfTrue="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="7" priority="38" stopIfTrue="1" operator="lessThanOrEqual">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P4:P14">
-    <cfRule type="cellIs" dxfId="2" priority="15" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="39" stopIfTrue="1" operator="equal">
       <formula>"buy"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4:M14">
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="30" operator="greaterThan">
       <formula>$N4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4:M14">
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="29" operator="lessThan">
       <formula>$N4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:K14">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
+        <cfvo type="percentile" val="10"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="percentile" val="90"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFCFCFF"/>
         <color rgb="FF63BE7B"/>

</xml_diff>

<commit_message>
updates and rename main to optimize portfolio
</commit_message>
<xml_diff>
--- a/Portfolio Optimization Tool.xlsx
+++ b/Portfolio Optimization Tool.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanlupinski/Documents/GitHub/Portfolio-Optimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AFD075D-EFDF-3041-8FCB-0C77F5024BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6EB5088-2980-3C44-9E47-3B82A0104277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,6 +22,8 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Portfolio!$B$2:$Q$16</definedName>
     <definedName name="_xlchart.v1.0" hidden="1">Portfolio!$B$4:$F$15</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">Portfolio!$F$4:$F$15</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Portfolio!$B$4:$F$15</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Portfolio!$F$4:$F$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1235,10 +1237,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:strDim>
       <cx:numDim type="size">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2022,9 +2024,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2062,7 +2064,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2168,7 +2170,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2310,7 +2312,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2320,9 +2322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -2353,11 +2353,11 @@
       <c r="J2" s="45"/>
       <c r="K2" s="46">
         <f>INDEX('Price Data'!$A$2:$A$265,COUNT('Price Data'!$A$2:$A$265))</f>
-        <v>45106</v>
+        <v>45351</v>
       </c>
       <c r="L2" s="47">
         <f>INDEX('Price Data'!$L$2:$L$255,COUNT('Price Data'!$L$2:$L$255))</f>
-        <v>40.330001831054602</v>
+        <v>41.020000457763601</v>
       </c>
       <c r="M2" s="56" t="s">
         <v>0</v>
@@ -2440,39 +2440,39 @@
       </c>
       <c r="G4" s="42">
         <f t="shared" ref="G4:G15" si="1">F4*$P$17</f>
-        <v>20000</v>
+        <v>37800</v>
       </c>
       <c r="H4" s="25">
         <f>'Performance Data'!$E$2</f>
-        <v>5.1291490392931099E-2</v>
+        <v>9.9969896936617605E-2</v>
       </c>
       <c r="I4" s="2">
         <f>'Performance Data'!$E$3</f>
-        <v>2.45253439784902E-2</v>
+        <v>0.21662284148365599</v>
       </c>
       <c r="J4" s="2">
         <f>'Performance Data'!$E$4</f>
-        <v>-1.7999480157139799E-2</v>
+        <v>0.244286706271057</v>
       </c>
       <c r="K4" s="2">
         <f>'Performance Data'!$E$5</f>
-        <v>6.4961294836280895E-2</v>
+        <v>0.32821832792835498</v>
       </c>
       <c r="L4" s="10">
         <f t="shared" ref="L4:L14" si="2">AVERAGE(H4:K4)</f>
-        <v>3.0694662262640598E-2</v>
+        <v>0.2222744431549214</v>
       </c>
       <c r="M4" s="3">
         <f t="shared" ref="M4:M14" si="3">_xlfn.RANK.EQ(L4,$L$4:$L$14,0)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N4" s="11">
         <f>INDEX('Price Data'!$E$2:$E$265,COUNT('Price Data'!$E$2:$E$265))</f>
-        <v>142.44999694824199</v>
+        <v>182.21000671386699</v>
       </c>
       <c r="O4" s="12">
         <f>'200D SMA'!$E$2</f>
-        <v>141.878150177001</v>
+        <v>149.34149986266999</v>
       </c>
       <c r="P4" s="5" t="str">
         <f t="shared" ref="P4:P14" si="4">IF(N4&gt;O4,"yes","no")</f>
@@ -2504,27 +2504,27 @@
       </c>
       <c r="G5" s="42">
         <f t="shared" si="1"/>
-        <v>20000</v>
+        <v>37800</v>
       </c>
       <c r="H5" s="25">
         <f>'Performance Data'!$K$2</f>
-        <v>4.5484821768132899E-2</v>
+        <v>3.3355428895916799E-2</v>
       </c>
       <c r="I5" s="2">
         <f>'Performance Data'!$K$3</f>
-        <v>2.0201240126006902E-2</v>
+        <v>9.5396182037539898E-2</v>
       </c>
       <c r="J5" s="2">
         <f>'Performance Data'!$K$4</f>
-        <v>9.9917190501552702E-3</v>
+        <v>0.100397674187316</v>
       </c>
       <c r="K5" s="2">
         <f>'Performance Data'!$K$5</f>
-        <v>9.0234970224636099E-2</v>
+        <v>0.14564250930258399</v>
       </c>
       <c r="L5" s="10">
         <f t="shared" si="2"/>
-        <v>4.1478187792232793E-2</v>
+        <v>9.3697948605839174E-2</v>
       </c>
       <c r="M5" s="3">
         <f t="shared" si="3"/>
@@ -2532,11 +2532,11 @@
       </c>
       <c r="N5" s="11">
         <f>INDEX('Price Data'!$K$2:$K$265,COUNT('Price Data'!$K$2:$K$265))</f>
-        <v>140.89999389648401</v>
+        <v>155.83000183105401</v>
       </c>
       <c r="O5" s="12">
         <f>'200D SMA'!$K$2</f>
-        <v>138.31995002746501</v>
+        <v>143.42199981689399</v>
       </c>
       <c r="P5" s="7" t="str">
         <f t="shared" si="4"/>
@@ -2568,39 +2568,39 @@
       </c>
       <c r="G6" s="42">
         <f t="shared" si="1"/>
-        <v>20000</v>
+        <v>37800</v>
       </c>
       <c r="H6" s="25">
         <f>'Performance Data'!$G$2</f>
-        <v>2.2044847414643499E-2</v>
+        <v>3.16971568378841E-2</v>
       </c>
       <c r="I6" s="2">
         <f>'Performance Data'!$G$3</f>
-        <v>5.7975977467099498E-3</v>
+        <v>6.4376062783104704E-2</v>
       </c>
       <c r="J6" s="2">
         <f>'Performance Data'!$G$4</f>
-        <v>7.5036096712882E-2</v>
+        <v>7.74593854398406E-2</v>
       </c>
       <c r="K6" s="2">
         <f>'Performance Data'!$G$5</f>
-        <v>9.8248330983337698E-2</v>
+        <v>0.13091150270959601</v>
       </c>
       <c r="L6" s="10">
         <f t="shared" si="2"/>
-        <v>5.0281718214393284E-2</v>
+        <v>7.6111026942606352E-2</v>
       </c>
       <c r="M6" s="3">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N6" s="11">
         <f>INDEX('Price Data'!$G$2:$G$265,COUNT('Price Data'!$G$2:$G$265))</f>
-        <v>53.779998779296797</v>
+        <v>56.959999084472599</v>
       </c>
       <c r="O6" s="12">
         <f>'200D SMA'!$G$2</f>
-        <v>51.4951998710632</v>
+        <v>54.091399745941096</v>
       </c>
       <c r="P6" s="7" t="str">
         <f t="shared" si="4"/>
@@ -2632,27 +2632,27 @@
       </c>
       <c r="G7" s="42">
         <f t="shared" si="1"/>
-        <v>20000</v>
+        <v>37800</v>
       </c>
       <c r="H7" s="25">
         <f>'Performance Data'!$L$2</f>
-        <v>3.2778556184434399E-2</v>
+        <v>3.4813347360333098E-2</v>
       </c>
       <c r="I7" s="2">
         <f>'Performance Data'!$L$3</f>
-        <v>-1.73266564803031E-3</v>
+        <v>3.1320031312261902E-2</v>
       </c>
       <c r="J7" s="2">
         <f>'Performance Data'!$L$4</f>
-        <v>3.5381492956410597E-2</v>
+        <v>4.2297730559299002E-2</v>
       </c>
       <c r="K7" s="2">
         <f>'Performance Data'!$L$5</f>
-        <v>-1.85396300287743E-3</v>
+        <v>7.8258237161627303E-2</v>
       </c>
       <c r="L7" s="10">
         <f t="shared" si="2"/>
-        <v>1.6143355122484312E-2</v>
+        <v>4.6672336598380326E-2</v>
       </c>
       <c r="M7" s="3">
         <f t="shared" si="3"/>
@@ -2660,11 +2660,11 @@
       </c>
       <c r="N7" s="11">
         <f>INDEX('Price Data'!$L$2:$L$265,COUNT('Price Data'!$L$2:$L$265))</f>
-        <v>40.330001831054602</v>
+        <v>41.020000457763601</v>
       </c>
       <c r="O7" s="12">
         <f>'200D SMA'!$L$2</f>
-        <v>39.626099967956499</v>
+        <v>40.295900001525801</v>
       </c>
       <c r="P7" s="7" t="str">
         <f t="shared" si="4"/>
@@ -2700,35 +2700,35 @@
       </c>
       <c r="H8" s="25">
         <f>'Performance Data'!$F$2</f>
-        <v>-1.03060833909124E-2</v>
+        <v>-1.44393918347506E-2</v>
       </c>
       <c r="I8" s="2">
         <f>'Performance Data'!$F$3</f>
-        <v>-1.6123223557787801E-2</v>
+        <v>2.5661457336266701E-2</v>
       </c>
       <c r="J8" s="2">
         <f>'Performance Data'!$F$4</f>
-        <v>2.4057340063055401E-2</v>
+        <v>4.0440572609490001E-2</v>
       </c>
       <c r="K8" s="2">
         <f>'Performance Data'!$F$5</f>
-        <v>1.05608216728496E-2</v>
+        <v>6.4192635500639E-2</v>
       </c>
       <c r="L8" s="10">
         <f t="shared" si="2"/>
-        <v>2.0472136968012001E-3</v>
+        <v>2.8963818402911276E-2</v>
       </c>
       <c r="M8" s="3">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N8" s="11">
         <f>INDEX('Price Data'!$F$2:$F$265,COUNT('Price Data'!$F$2:$F$265))</f>
-        <v>78.699996948242102</v>
+        <v>79.790000915527301</v>
       </c>
       <c r="O8" s="12">
         <f>'200D SMA'!$F$2</f>
-        <v>78.425199928283604</v>
+        <v>78.316349906921303</v>
       </c>
       <c r="P8" s="7" t="str">
         <f t="shared" si="4"/>
@@ -2764,23 +2764,23 @@
       </c>
       <c r="H9" s="25">
         <f>'Performance Data'!$H$2</f>
-        <v>-1.5125403758072401E-2</v>
+        <v>-2.32728065760055E-2</v>
       </c>
       <c r="I9" s="2">
         <f>'Performance Data'!$H$3</f>
-        <v>-3.7666472796377602E-2</v>
+        <v>3.8119506935142697E-2</v>
       </c>
       <c r="J9" s="2">
         <f>'Performance Data'!$H$4</f>
-        <v>2.8059952696565599E-2</v>
+        <v>-1.7306641113679E-3</v>
       </c>
       <c r="K9" s="2">
         <f>'Performance Data'!$H$5</f>
-        <v>-8.2289980734325904E-2</v>
+        <v>-2.9391567247999802E-2</v>
       </c>
       <c r="L9" s="10">
         <f t="shared" si="2"/>
-        <v>-2.6755476148052577E-2</v>
+        <v>-4.0688827500576265E-3</v>
       </c>
       <c r="M9" s="3">
         <f t="shared" si="3"/>
@@ -2788,11 +2788,11 @@
       </c>
       <c r="N9" s="11">
         <f>INDEX('Price Data'!$H$2:$H$265,COUNT('Price Data'!$H$2:$H$265))</f>
-        <v>62.889999389648402</v>
+        <v>58.840000152587798</v>
       </c>
       <c r="O9" s="12">
         <f>'200D SMA'!$H$2</f>
-        <v>63.6645500183105</v>
+        <v>59.1889000701904</v>
       </c>
       <c r="P9" s="7" t="str">
         <f t="shared" si="4"/>
@@ -2828,35 +2828,35 @@
       </c>
       <c r="H10" s="25">
         <f>'Performance Data'!$B$2</f>
-        <v>-4.45123340187825E-3</v>
+        <v>-5.3884137192383701E-3</v>
       </c>
       <c r="I10" s="2">
         <f>'Performance Data'!$B$3</f>
-        <v>-9.4362220951671395E-4</v>
+        <v>2.0610385919621801E-2</v>
       </c>
       <c r="J10" s="2">
         <f>'Performance Data'!$B$4</f>
-        <v>3.3056465146963102E-2</v>
+        <v>3.5652626583980898E-2</v>
       </c>
       <c r="K10" s="2">
         <f>'Performance Data'!$B$5</f>
-        <v>-3.15051651330722E-4</v>
+        <v>6.6803642820775E-2</v>
       </c>
       <c r="L10" s="10">
         <f t="shared" si="2"/>
-        <v>6.8366394710593541E-3</v>
+        <v>2.9419560401284833E-2</v>
       </c>
       <c r="M10" s="3">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N10" s="11">
         <f>INDEX('Price Data'!$B$2:$B$265,COUNT('Price Data'!$B$2:$B$265))</f>
-        <v>48.810001373291001</v>
+        <v>48.7299995422363</v>
       </c>
       <c r="O10" s="12">
         <f>'200D SMA'!$B$2</f>
-        <v>48.426050033569297</v>
+        <v>48.6257500457763</v>
       </c>
       <c r="P10" s="7" t="str">
         <f t="shared" si="4"/>
@@ -2892,23 +2892,23 @@
       </c>
       <c r="H11" s="25">
         <f>'Performance Data'!$J$2</f>
-        <v>-1.07012975589151E-2</v>
+        <v>-2.0956053281698801E-3</v>
       </c>
       <c r="I11" s="2">
         <f>'Performance Data'!$J$3</f>
-        <v>-1.6104166912779199E-2</v>
+        <v>1.34366668298444E-2</v>
       </c>
       <c r="J11" s="2">
         <f>'Performance Data'!$J$4</f>
-        <v>7.2767560808448799E-3</v>
+        <v>2.5991663553750901E-2</v>
       </c>
       <c r="K11" s="2">
         <f>'Performance Data'!$J$5</f>
-        <v>-6.8615225631711799E-3</v>
+        <v>4.5033484142287902E-2</v>
       </c>
       <c r="L11" s="10">
         <f t="shared" si="2"/>
-        <v>-6.5975577385051498E-3</v>
+        <v>2.0591552299428328E-2</v>
       </c>
       <c r="M11" s="3">
         <f t="shared" si="3"/>
@@ -2916,15 +2916,15 @@
       </c>
       <c r="N11" s="11">
         <f>INDEX('Price Data'!$J$2:$J$265,COUNT('Price Data'!$J$2:$J$265))</f>
-        <v>47.369998931884702</v>
+        <v>47.619998931884702</v>
       </c>
       <c r="O11" s="12">
         <f>'200D SMA'!$J$2</f>
-        <v>47.5597500419616</v>
+        <v>47.386900024413997</v>
       </c>
       <c r="P11" s="7" t="str">
         <f t="shared" si="4"/>
-        <v>no</v>
+        <v>yes</v>
       </c>
       <c r="Q11" s="6" t="str">
         <f t="shared" si="5"/>
@@ -2956,23 +2956,23 @@
       </c>
       <c r="H12" s="25">
         <f>'Performance Data'!$C$2</f>
-        <v>2.08617237069166E-2</v>
+        <v>-1.5226160042523499E-2</v>
       </c>
       <c r="I12" s="2">
         <f>'Performance Data'!$C$3</f>
-        <v>-5.1811270180917399E-2</v>
+        <v>-3.5106798144615203E-2</v>
       </c>
       <c r="J12" s="2">
         <f>'Performance Data'!$C$4</f>
-        <v>-8.6815392404296102E-2</v>
+        <v>-6.1789481547861201E-2</v>
       </c>
       <c r="K12" s="2">
         <f>'Performance Data'!$C$5</f>
-        <v>-0.14992818301996</v>
+        <v>-2.9015272441596001E-2</v>
       </c>
       <c r="L12" s="10">
         <f t="shared" si="2"/>
-        <v>-6.6923280474564223E-2</v>
+        <v>-3.5284428044148976E-2</v>
       </c>
       <c r="M12" s="3">
         <f t="shared" si="3"/>
@@ -2980,11 +2980,11 @@
       </c>
       <c r="N12" s="11">
         <f>INDEX('Price Data'!$C$2:$C$265,COUNT('Price Data'!$C$2:$C$265))</f>
-        <v>22.5100002288818</v>
+        <v>21.9899997711181</v>
       </c>
       <c r="O12" s="12">
         <f>'200D SMA'!$C$2</f>
-        <v>24.1112500095367</v>
+        <v>23.500049962997402</v>
       </c>
       <c r="P12" s="7" t="str">
         <f t="shared" si="4"/>
@@ -3008,47 +3008,47 @@
       </c>
       <c r="E13" s="29">
         <f t="shared" si="6"/>
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F13" s="30">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G13" s="42">
         <f t="shared" si="1"/>
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="H13" s="25">
         <f>'Performance Data'!$D$2</f>
-        <v>-2.8225785363601499E-2</v>
+        <v>4.1569197307056403E-3</v>
       </c>
       <c r="I13" s="2">
         <f>'Performance Data'!$D$3</f>
-        <v>-3.2646439413326497E-2</v>
+        <v>2.85419324697655E-3</v>
       </c>
       <c r="J13" s="2">
         <f>'Performance Data'!$D$4</f>
-        <v>4.5099779312210098E-2</v>
+        <v>5.1700721792621702E-2</v>
       </c>
       <c r="K13" s="2">
         <f>'Performance Data'!$D$5</f>
-        <v>5.3628681986011797E-2</v>
+        <v>0.116406779847775</v>
       </c>
       <c r="L13" s="10">
         <f t="shared" si="2"/>
-        <v>9.4640591303234746E-3</v>
+        <v>4.3779653654519725E-2</v>
       </c>
       <c r="M13" s="3">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N13" s="11">
         <f>INDEX('Price Data'!$D$2:$D$265,COUNT('Price Data'!$D$2:$D$265))</f>
-        <v>36.150001525878899</v>
+        <v>38.650001525878899</v>
       </c>
       <c r="O13" s="12">
         <f>'200D SMA'!$D$2</f>
-        <v>35.119449939727701</v>
+        <v>37.2485998535156</v>
       </c>
       <c r="P13" s="7" t="str">
         <f t="shared" si="4"/>
@@ -3056,7 +3056,7 @@
       </c>
       <c r="Q13" s="6" t="str">
         <f t="shared" si="5"/>
-        <v>add 20%</v>
+        <v>n/a</v>
       </c>
     </row>
     <row r="14" spans="2:17" ht="17" thickBot="1">
@@ -3072,55 +3072,55 @@
       </c>
       <c r="E14" s="29">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="F14" s="30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G14" s="42">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>37800</v>
       </c>
       <c r="H14" s="26">
         <f>'Performance Data'!$I$2</f>
-        <v>3.8749980926513397E-2</v>
+        <v>1.9787861177576801E-2</v>
       </c>
       <c r="I14" s="17">
         <f>'Performance Data'!$I$3</f>
-        <v>7.2251394427103001E-4</v>
+        <v>5.9647902597001097E-2</v>
       </c>
       <c r="J14" s="17">
         <f>'Performance Data'!$I$4</f>
-        <v>1.7615678860427499E-2</v>
+        <v>6.1515332328163197E-2</v>
       </c>
       <c r="K14" s="17">
         <f>'Performance Data'!$I$5</f>
-        <v>-5.5633365887086499E-2</v>
+        <v>4.2014912252332698E-2</v>
       </c>
       <c r="L14" s="18">
         <f t="shared" si="2"/>
-        <v>3.6370196103135792E-4</v>
+        <v>4.5741502088768447E-2</v>
       </c>
       <c r="M14" s="4">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="N14" s="16">
         <f>INDEX('Price Data'!$I$2:$I$265,COUNT('Price Data'!$I$2:$I$265))</f>
-        <v>83.099998474121094</v>
+        <v>85.550003051757798</v>
       </c>
       <c r="O14" s="13">
         <f>'200D SMA'!$I$2</f>
-        <v>83.740399971008301</v>
+        <v>81.865499992370601</v>
       </c>
       <c r="P14" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>no</v>
+        <v>yes</v>
       </c>
       <c r="Q14" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>n/a</v>
+        <v>add 20%</v>
       </c>
     </row>
     <row r="15" spans="2:17" ht="17" thickBot="1">
@@ -3165,7 +3165,7 @@
       </c>
       <c r="G16" s="43">
         <f>SUM(G4:G15)</f>
-        <v>100000</v>
+        <v>189000</v>
       </c>
       <c r="N16" s="54" t="s">
         <v>53</v>
@@ -3182,7 +3182,7 @@
       </c>
       <c r="O17" s="49"/>
       <c r="P17" s="52">
-        <v>100000</v>
+        <v>189000</v>
       </c>
       <c r="Q17" s="53"/>
     </row>
@@ -3327,7 +3327,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L261"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:L2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -3377,40 +3379,40 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="23">
-        <v>45106</v>
+        <v>45351</v>
       </c>
       <c r="B2">
-        <v>48.810001373291001</v>
+        <v>48.7299995422363</v>
       </c>
       <c r="C2">
-        <v>22.5100002288818</v>
+        <v>21.9899997711181</v>
       </c>
       <c r="D2">
-        <v>36.150001525878899</v>
+        <v>38.650001525878899</v>
       </c>
       <c r="E2">
-        <v>142.44999694824199</v>
+        <v>182.21000671386699</v>
       </c>
       <c r="F2">
-        <v>78.699996948242102</v>
+        <v>79.790000915527301</v>
       </c>
       <c r="G2">
-        <v>53.779998779296797</v>
+        <v>56.959999084472599</v>
       </c>
       <c r="H2">
-        <v>62.889999389648402</v>
+        <v>58.840000152587798</v>
       </c>
       <c r="I2">
-        <v>83.099998474121094</v>
+        <v>85.550003051757798</v>
       </c>
       <c r="J2">
-        <v>47.369998931884702</v>
+        <v>47.619998931884702</v>
       </c>
       <c r="K2">
-        <v>140.89999389648401</v>
+        <v>155.83000183105401</v>
       </c>
       <c r="L2">
-        <v>40.330001831054602</v>
+        <v>41.020000457763601</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -4193,7 +4195,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4244,40 +4246,40 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="23">
-        <v>45106</v>
+        <v>45351</v>
       </c>
       <c r="B2">
-        <v>48.426050033569297</v>
+        <v>48.6257500457763</v>
       </c>
       <c r="C2">
-        <v>24.1112500095367</v>
+        <v>23.500049962997402</v>
       </c>
       <c r="D2">
-        <v>35.119449939727701</v>
+        <v>37.2485998535156</v>
       </c>
       <c r="E2">
-        <v>141.878150177001</v>
+        <v>149.34149986266999</v>
       </c>
       <c r="F2">
-        <v>78.425199928283604</v>
+        <v>78.316349906921303</v>
       </c>
       <c r="G2">
-        <v>51.4951998710632</v>
+        <v>54.091399745941096</v>
       </c>
       <c r="H2">
-        <v>63.6645500183105</v>
+        <v>59.1889000701904</v>
       </c>
       <c r="I2">
-        <v>83.740399971008301</v>
+        <v>81.865499992370601</v>
       </c>
       <c r="J2">
-        <v>47.5597500419616</v>
+        <v>47.386900024413997</v>
       </c>
       <c r="K2">
-        <v>138.31995002746501</v>
+        <v>143.42199981689399</v>
       </c>
       <c r="L2">
-        <v>39.626099967956499</v>
+        <v>40.295900001525801</v>
       </c>
     </row>
   </sheetData>
@@ -4350,40 +4352,40 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="23">
-        <v>45106</v>
+        <v>45351</v>
       </c>
       <c r="B2">
-        <v>-4.45123340187825E-3</v>
+        <v>-5.3884137192383701E-3</v>
       </c>
       <c r="C2">
-        <v>2.08617237069166E-2</v>
+        <v>-1.5226160042523499E-2</v>
       </c>
       <c r="D2">
-        <v>-2.8225785363601499E-2</v>
+        <v>4.1569197307056403E-3</v>
       </c>
       <c r="E2">
-        <v>5.1291490392931099E-2</v>
+        <v>9.9969896936617605E-2</v>
       </c>
       <c r="F2">
-        <v>-1.03060833909124E-2</v>
+        <v>-1.44393918347506E-2</v>
       </c>
       <c r="G2">
-        <v>2.2044847414643499E-2</v>
+        <v>3.16971568378841E-2</v>
       </c>
       <c r="H2">
-        <v>-1.5125403758072401E-2</v>
+        <v>-2.32728065760055E-2</v>
       </c>
       <c r="I2">
-        <v>3.8749980926513397E-2</v>
+        <v>1.9787861177576801E-2</v>
       </c>
       <c r="J2">
-        <v>-1.07012975589151E-2</v>
+        <v>-2.0956053281698801E-3</v>
       </c>
       <c r="K2">
-        <v>4.5484821768132899E-2</v>
+        <v>3.3355428895916799E-2</v>
       </c>
       <c r="L2">
-        <v>3.2778556184434399E-2</v>
+        <v>3.4813347360333098E-2</v>
       </c>
       <c r="M2" t="s">
         <v>39</v>
@@ -4391,40 +4393,40 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="23">
-        <v>45106</v>
+        <v>45351</v>
       </c>
       <c r="B3">
-        <v>-9.4362220951671395E-4</v>
+        <v>2.0610385919621801E-2</v>
       </c>
       <c r="C3">
-        <v>-5.1811270180917399E-2</v>
+        <v>-3.5106798144615203E-2</v>
       </c>
       <c r="D3">
-        <v>-3.2646439413326497E-2</v>
+        <v>2.85419324697655E-3</v>
       </c>
       <c r="E3">
-        <v>2.45253439784902E-2</v>
+        <v>0.21662284148365599</v>
       </c>
       <c r="F3">
-        <v>-1.6123223557787801E-2</v>
+        <v>2.5661457336266701E-2</v>
       </c>
       <c r="G3">
-        <v>5.7975977467099498E-3</v>
+        <v>6.4376062783104704E-2</v>
       </c>
       <c r="H3">
-        <v>-3.7666472796377602E-2</v>
+        <v>3.8119506935142697E-2</v>
       </c>
       <c r="I3">
-        <v>7.2251394427103001E-4</v>
+        <v>5.9647902597001097E-2</v>
       </c>
       <c r="J3">
-        <v>-1.6104166912779199E-2</v>
+        <v>1.34366668298444E-2</v>
       </c>
       <c r="K3">
-        <v>2.0201240126006902E-2</v>
+        <v>9.5396182037539898E-2</v>
       </c>
       <c r="L3">
-        <v>-1.73266564803031E-3</v>
+        <v>3.1320031312261902E-2</v>
       </c>
       <c r="M3" t="s">
         <v>40</v>
@@ -4432,40 +4434,40 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="23">
-        <v>45106</v>
+        <v>45351</v>
       </c>
       <c r="B4">
-        <v>3.3056465146963102E-2</v>
+        <v>3.5652626583980898E-2</v>
       </c>
       <c r="C4">
-        <v>-8.6815392404296102E-2</v>
+        <v>-6.1789481547861201E-2</v>
       </c>
       <c r="D4">
-        <v>4.5099779312210098E-2</v>
+        <v>5.1700721792621702E-2</v>
       </c>
       <c r="E4">
-        <v>-1.7999480157139799E-2</v>
+        <v>0.244286706271057</v>
       </c>
       <c r="F4">
-        <v>2.4057340063055401E-2</v>
+        <v>4.0440572609490001E-2</v>
       </c>
       <c r="G4">
-        <v>7.5036096712882E-2</v>
+        <v>7.74593854398406E-2</v>
       </c>
       <c r="H4">
-        <v>2.8059952696565599E-2</v>
+        <v>-1.7306641113679E-3</v>
       </c>
       <c r="I4">
-        <v>1.7615678860427499E-2</v>
+        <v>6.1515332328163197E-2</v>
       </c>
       <c r="J4">
-        <v>7.2767560808448799E-3</v>
+        <v>2.5991663553750901E-2</v>
       </c>
       <c r="K4">
-        <v>9.9917190501552702E-3</v>
+        <v>0.100397674187316</v>
       </c>
       <c r="L4">
-        <v>3.5381492956410597E-2</v>
+        <v>4.2297730559299002E-2</v>
       </c>
       <c r="M4" t="s">
         <v>41</v>
@@ -4473,40 +4475,40 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="23">
-        <v>45106</v>
+        <v>45351</v>
       </c>
       <c r="B5">
-        <v>-3.15051651330722E-4</v>
+        <v>6.6803642820775E-2</v>
       </c>
       <c r="C5">
-        <v>-0.14992818301996</v>
+        <v>-2.9015272441596001E-2</v>
       </c>
       <c r="D5">
-        <v>5.3628681986011797E-2</v>
+        <v>0.116406779847775</v>
       </c>
       <c r="E5">
-        <v>6.4961294836280895E-2</v>
+        <v>0.32821832792835498</v>
       </c>
       <c r="F5">
-        <v>1.05608216728496E-2</v>
+        <v>6.4192635500639E-2</v>
       </c>
       <c r="G5">
-        <v>9.8248330983337698E-2</v>
+        <v>0.13091150270959601</v>
       </c>
       <c r="H5">
-        <v>-8.2289980734325904E-2</v>
+        <v>-2.9391567247999802E-2</v>
       </c>
       <c r="I5">
-        <v>-5.5633365887086499E-2</v>
+        <v>4.2014912252332698E-2</v>
       </c>
       <c r="J5">
-        <v>-6.8615225631711799E-3</v>
+        <v>4.5033484142287902E-2</v>
       </c>
       <c r="K5">
-        <v>9.0234970224636099E-2</v>
+        <v>0.14564250930258399</v>
       </c>
       <c r="L5">
-        <v>-1.85396300287743E-3</v>
+        <v>7.8258237161627303E-2</v>
       </c>
       <c r="M5" t="s">
         <v>42</v>

</xml_diff>